<commit_message>
version 2 done based on the picklist is old one
</commit_message>
<xml_diff>
--- a/public/bulk-bag-sheet-sample.xlsx
+++ b/public/bulk-bag-sheet-sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7EA6649-AFF4-4803-A132-3F2DA8DF00C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{066D0855-E7B6-46B5-867C-C176DF967A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="132" windowWidth="22932" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>SELECT Store Name</t>
   </si>
@@ -51,6 +52,9 @@
   </si>
   <si>
     <t>Warehouse</t>
+  </si>
+  <si>
+    <t>CPC</t>
   </si>
 </sst>
 </file>
@@ -194,7 +198,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -541,9 +545,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -926,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I337"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -936,9 +941,10 @@
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15">
@@ -963,16 +969,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="15">
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="15">
       <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="15">
       <c r="G4" s="1"/>

</xml_diff>